<commit_message>
implement the cell color component to display the marked student answer sheet
</commit_message>
<xml_diff>
--- a/src/main/resources/files/student_sheet/answer_sheet.xlsx
+++ b/src/main/resources/files/student_sheet/answer_sheet.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_0_dev\projects\poc-excel-compare\src\main\resources\files\instructor_sheet\"/>
     </mc:Choice>
@@ -181,8 +181,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
@@ -246,7 +246,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -277,6 +277,42 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="42"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="42"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="48"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="48"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="48"/>
+        <bgColor indexed="48"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="24">
     <border>
@@ -536,7 +572,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="118">
+  <cellXfs count="253">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="2" fillId="4" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="3" fillId="4" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -811,6 +847,141 @@
     <xf numFmtId="164" fontId="4" fillId="5" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="true"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1166,15 +1337,15 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.69921875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.69921875" style="4" customWidth="1"/>
-    <col min="2" max="2" width="9.69921875" style="4" customWidth="1"/>
-    <col min="3" max="3" width="2.19921875" style="4" customWidth="1"/>
-    <col min="4" max="4" width="6.19921875" style="4" customWidth="1"/>
-    <col min="5" max="5" width="10.59765625" style="4" customWidth="1"/>
-    <col min="6" max="6" width="6.19921875" style="4" customWidth="1"/>
-    <col min="7" max="7" width="13.09765625" style="4" customWidth="1"/>
-    <col min="8" max="8" width="10.19921875" style="4" customWidth="1"/>
-    <col min="9" max="16384" width="8.69921875" style="4"/>
+    <col min="1" max="1" customWidth="true" style="4" width="26.69921875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="4" width="9.69921875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="4" width="2.19921875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="4" width="6.19921875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="4" width="10.59765625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="4" width="6.19921875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="4" width="13.09765625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="4" width="10.19921875" collapsed="true"/>
+    <col min="9" max="16384" style="4" width="8.69921875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.6">
@@ -1240,7 +1411,7 @@
       <c r="B6" s="9"/>
       <c r="C6" s="9"/>
       <c r="D6" s="9"/>
-      <c r="E6" s="54">
+      <c r="E6" s="201">
         <v>30</v>
       </c>
       <c r="F6" s="9"/>
@@ -1254,7 +1425,7 @@
       <c r="B7" s="9"/>
       <c r="C7" s="9"/>
       <c r="D7" s="9"/>
-      <c r="E7" s="59">
+      <c r="E7" s="204">
         <v>0.8</v>
       </c>
       <c r="F7" s="9"/>
@@ -1268,7 +1439,7 @@
       <c r="B8" s="9"/>
       <c r="C8" s="9"/>
       <c r="D8" s="9"/>
-      <c r="E8" s="59">
+      <c r="E8" s="207">
         <v>0.5</v>
       </c>
       <c r="F8" s="9"/>
@@ -1282,7 +1453,7 @@
       <c r="B9" s="9"/>
       <c r="C9" s="9"/>
       <c r="D9" s="9"/>
-      <c r="E9" s="54">
+      <c r="E9" s="210">
         <v>72</v>
       </c>
       <c r="F9" s="9"/>
@@ -1296,7 +1467,7 @@
       <c r="B10" s="9"/>
       <c r="C10" s="9"/>
       <c r="D10" s="9"/>
-      <c r="E10" s="54">
+      <c r="E10" s="219">
         <v>35</v>
       </c>
       <c r="F10" s="9"/>
@@ -1310,7 +1481,7 @@
       <c r="B11" s="9"/>
       <c r="C11" s="9"/>
       <c r="D11" s="9"/>
-      <c r="E11" s="58">
+      <c r="E11" s="213">
         <v>0.2</v>
       </c>
       <c r="F11" s="9"/>
@@ -1324,7 +1495,7 @@
       <c r="B12" s="9"/>
       <c r="C12" s="9"/>
       <c r="D12" s="9"/>
-      <c r="E12" s="59">
+      <c r="E12" s="231">
         <v>0.4</v>
       </c>
       <c r="F12" s="9"/>
@@ -1360,7 +1531,7 @@
       <c r="B15" s="9"/>
       <c r="C15" s="9"/>
       <c r="D15" s="9"/>
-      <c r="E15" s="60"/>
+      <c r="E15" s="238"/>
       <c r="F15" s="9"/>
       <c r="G15" s="9"/>
       <c r="H15" s="69"/>
@@ -1372,7 +1543,7 @@
       <c r="B16" s="9"/>
       <c r="C16" s="9"/>
       <c r="D16" s="9"/>
-      <c r="E16" s="60">
+      <c r="E16" s="249">
         <v>8400</v>
       </c>
       <c r="F16" s="9"/>
@@ -1386,7 +1557,7 @@
       <c r="B17" s="9"/>
       <c r="C17" s="9"/>
       <c r="D17" s="9"/>
-      <c r="E17" s="54">
+      <c r="E17" s="243">
         <v>9000</v>
       </c>
       <c r="F17" s="9"/>
@@ -1422,7 +1593,7 @@
       <c r="B20" s="9"/>
       <c r="C20" s="9"/>
       <c r="D20" s="9"/>
-      <c r="E20" s="54">
+      <c r="E20" s="129">
         <v>17500</v>
       </c>
       <c r="F20" s="9"/>
@@ -1436,7 +1607,7 @@
       <c r="B21" s="13"/>
       <c r="C21" s="13"/>
       <c r="D21" s="13"/>
-      <c r="E21" s="61">
+      <c r="E21" s="162">
         <v>39600</v>
       </c>
       <c r="F21" s="9"/>
@@ -1611,7 +1782,7 @@
       <c r="A36" s="82" t="s">
         <v>20</v>
       </c>
-      <c r="B36" s="83">
+      <c r="B36" s="221">
         <f>E6</f>
         <v>30</v>
       </c>
@@ -1626,7 +1797,7 @@
       <c r="A37" s="82" t="s">
         <v>21</v>
       </c>
-      <c r="B37" s="83">
+      <c r="B37" s="224">
         <f>E9</f>
         <v>72</v>
       </c>
@@ -1641,7 +1812,7 @@
       <c r="A38" s="82" t="s">
         <v>10</v>
       </c>
-      <c r="B38" s="29">
+      <c r="B38" s="233">
         <f>SUM(B36:B37)</f>
         <v>102</v>
       </c>
@@ -1678,22 +1849,22 @@
       <c r="A41" s="82" t="s">
         <v>22</v>
       </c>
-      <c r="B41" s="83">
+      <c r="B41" s="251">
         <f>B43-B42</f>
         <v>67</v>
       </c>
       <c r="C41" s="84"/>
-      <c r="D41" s="86">
+      <c r="D41" s="120">
         <v>1</v>
       </c>
-      <c r="E41" s="83">
+      <c r="E41" s="143">
         <f>B41*D41</f>
         <v>67</v>
       </c>
-      <c r="F41" s="87">
+      <c r="F41" s="132">
         <v>1</v>
       </c>
-      <c r="G41" s="83">
+      <c r="G41" s="164">
         <f>B41*F41</f>
         <v>67</v>
       </c>
@@ -1703,24 +1874,24 @@
       <c r="A42" s="82" t="s">
         <v>23</v>
       </c>
-      <c r="B42" s="83">
+      <c r="B42" s="122">
         <f>E10</f>
         <v>35</v>
       </c>
       <c r="C42" s="84"/>
-      <c r="D42" s="86">
+      <c r="D42" s="146">
         <f>E11</f>
         <v>0.2</v>
       </c>
-      <c r="E42" s="83">
+      <c r="E42" s="134">
         <f>D42*B42</f>
         <v>7</v>
       </c>
-      <c r="F42" s="87">
+      <c r="F42" s="167">
         <f>E12</f>
         <v>0.4</v>
       </c>
-      <c r="G42" s="83">
+      <c r="G42" s="152">
         <f>B42*F42</f>
         <v>14</v>
       </c>
@@ -1730,18 +1901,18 @@
       <c r="A43" s="82" t="s">
         <v>10</v>
       </c>
-      <c r="B43" s="29">
+      <c r="B43" s="125">
         <f>B38</f>
         <v>102</v>
       </c>
       <c r="C43" s="84"/>
-      <c r="D43" s="88"/>
-      <c r="E43" s="29">
+      <c r="D43" s="136"/>
+      <c r="E43" s="170">
         <f>SUM(E41:E42)</f>
         <v>74</v>
       </c>
-      <c r="F43" s="83"/>
-      <c r="G43" s="29">
+      <c r="F43" s="154"/>
+      <c r="G43" s="176">
         <f>SUM(G41:G42)</f>
         <v>81</v>
       </c>
@@ -1794,12 +1965,12 @@
       <c r="B47" s="80"/>
       <c r="C47" s="93"/>
       <c r="D47" s="9"/>
-      <c r="E47" s="34">
+      <c r="E47" s="182">
         <f>E16+E20</f>
         <v>25900</v>
       </c>
       <c r="F47" s="35"/>
-      <c r="G47" s="34">
+      <c r="G47" s="188">
         <f>E17+E21</f>
         <v>48600</v>
       </c>
@@ -1812,12 +1983,12 @@
       <c r="B48" s="80"/>
       <c r="C48" s="93"/>
       <c r="D48" s="9"/>
-      <c r="E48" s="37">
+      <c r="E48" s="179">
         <f>E43</f>
         <v>74</v>
       </c>
       <c r="F48" s="9"/>
-      <c r="G48" s="37">
+      <c r="G48" s="185">
         <f>G43</f>
         <v>81</v>
       </c>
@@ -1830,16 +2001,16 @@
       <c r="B49" s="80"/>
       <c r="C49" s="93"/>
       <c r="D49" s="9"/>
-      <c r="E49" s="38">
+      <c r="E49" s="191">
         <f>E47/E48</f>
         <v>350</v>
       </c>
       <c r="F49" s="39"/>
-      <c r="G49" s="38">
+      <c r="G49" s="197">
         <f>G47/G48</f>
         <v>600</v>
       </c>
-      <c r="H49" s="96">
+      <c r="H49" s="194">
         <f>SUM(E49:G49)</f>
         <v>950</v>
       </c>
@@ -1876,7 +2047,7 @@
       <c r="E52" s="80"/>
       <c r="F52" s="65"/>
       <c r="G52" s="80"/>
-      <c r="H52" s="98">
+      <c r="H52" s="215">
         <f>E16+E17</f>
         <v>17400</v>
       </c>
@@ -1891,7 +2062,7 @@
       <c r="E53" s="80"/>
       <c r="F53" s="65"/>
       <c r="G53" s="80"/>
-      <c r="H53" s="99">
+      <c r="H53" s="236">
         <f>E20+E21</f>
         <v>57100</v>
       </c>
@@ -1906,7 +2077,7 @@
       <c r="E54" s="80"/>
       <c r="F54" s="65"/>
       <c r="G54" s="80"/>
-      <c r="H54" s="100">
+      <c r="H54" s="227">
         <f>SUM(H52:H53)</f>
         <v>74500</v>
       </c>
@@ -1955,7 +2126,7 @@
       <c r="E58" s="80"/>
       <c r="F58" s="65"/>
       <c r="G58" s="80"/>
-      <c r="H58" s="98">
+      <c r="H58" s="245">
         <f>H49*G41</f>
         <v>63650</v>
       </c>
@@ -1991,7 +2162,7 @@
       <c r="D61" s="65"/>
       <c r="E61" s="80"/>
       <c r="F61" s="65"/>
-      <c r="G61" s="102">
+      <c r="G61" s="149">
         <f>E42*E49</f>
         <v>2450</v>
       </c>
@@ -2006,11 +2177,11 @@
       <c r="D62" s="65"/>
       <c r="E62" s="80"/>
       <c r="F62" s="104"/>
-      <c r="G62" s="47">
+      <c r="G62" s="140">
         <f>G42*G49</f>
         <v>8400</v>
       </c>
-      <c r="H62" s="105">
+      <c r="H62" s="173">
         <f>SUM(G61:G62)</f>
         <v>10850</v>
       </c>
@@ -2025,7 +2196,7 @@
       <c r="E63" s="80"/>
       <c r="F63" s="106"/>
       <c r="G63" s="80"/>
-      <c r="H63" s="100">
+      <c r="H63" s="158">
         <f>SUM(H58:H62)</f>
         <v>74500</v>
       </c>
@@ -2056,15 +2227,15 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.69921875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.69921875" style="4" customWidth="1"/>
-    <col min="2" max="2" width="9.69921875" style="4" customWidth="1"/>
-    <col min="3" max="3" width="2.19921875" style="4" customWidth="1"/>
-    <col min="4" max="4" width="6.19921875" style="4" customWidth="1"/>
-    <col min="5" max="5" width="10.59765625" style="4" customWidth="1"/>
-    <col min="6" max="6" width="6.19921875" style="4" customWidth="1"/>
-    <col min="7" max="7" width="13.09765625" style="4" customWidth="1"/>
-    <col min="8" max="8" width="10.19921875" style="4" customWidth="1"/>
-    <col min="9" max="16384" width="8.69921875" style="4"/>
+    <col min="1" max="1" customWidth="true" style="4" width="26.69921875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="4" width="9.69921875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="4" width="2.19921875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="4" width="6.19921875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="4" width="10.59765625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="4" width="6.19921875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="4" width="13.09765625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="4" width="10.19921875" collapsed="true"/>
+    <col min="9" max="16384" style="4" width="8.69921875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.6">
@@ -2847,15 +3018,15 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.69921875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.69921875" style="4" customWidth="1"/>
-    <col min="2" max="2" width="9.69921875" style="4" customWidth="1"/>
-    <col min="3" max="3" width="2.19921875" style="4" customWidth="1"/>
-    <col min="4" max="4" width="6.19921875" style="4" customWidth="1"/>
-    <col min="5" max="5" width="10.59765625" style="4" customWidth="1"/>
-    <col min="6" max="6" width="6.19921875" style="4" customWidth="1"/>
-    <col min="7" max="7" width="13.09765625" style="4" customWidth="1"/>
-    <col min="8" max="8" width="10.19921875" style="4" customWidth="1"/>
-    <col min="9" max="16384" width="8.69921875" style="4"/>
+    <col min="1" max="1" customWidth="true" style="4" width="26.69921875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="4" width="9.69921875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="4" width="2.19921875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="4" width="6.19921875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="4" width="10.59765625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="4" width="6.19921875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="4" width="13.09765625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="4" width="10.19921875" collapsed="true"/>
+    <col min="9" max="16384" style="4" width="8.69921875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.6">

</xml_diff>

<commit_message>
Implement easy displaying marked paper process to the excel evaluation component
</commit_message>
<xml_diff>
--- a/src/main/resources/files/student_sheet/answer_sheet.xlsx
+++ b/src/main/resources/files/student_sheet/answer_sheet.xlsx
@@ -27,6 +27,241 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author/>
+  </authors>
+  <commentList>
+    <comment ref="D41" authorId="0">
+      <text>
+        <t>Partially Correct Answer given</t>
+      </text>
+    </comment>
+    <comment ref="B42" authorId="0">
+      <text>
+        <t>Correct Answer given</t>
+      </text>
+    </comment>
+    <comment ref="B43" authorId="0">
+      <text>
+        <t>Correct Answer given</t>
+      </text>
+    </comment>
+    <comment ref="E20" authorId="0">
+      <text>
+        <t>Partially Correct Answer given</t>
+      </text>
+    </comment>
+    <comment ref="F41" authorId="0">
+      <text>
+        <t>Partially Correct Answer given</t>
+      </text>
+    </comment>
+    <comment ref="E42" authorId="0">
+      <text>
+        <t>Correct Answer given</t>
+      </text>
+    </comment>
+    <comment ref="D43" authorId="0">
+      <text>
+        <t>Incorrect Answer given</t>
+      </text>
+    </comment>
+    <comment ref="G62" authorId="0">
+      <text>
+        <t>Correct Answer given</t>
+      </text>
+    </comment>
+    <comment ref="E41" authorId="0">
+      <text>
+        <t>Correct Answer given</t>
+      </text>
+    </comment>
+    <comment ref="D42" authorId="0">
+      <text>
+        <t>Correct Answer given</t>
+      </text>
+    </comment>
+    <comment ref="G61" authorId="0">
+      <text>
+        <t>Correct Answer given</t>
+      </text>
+    </comment>
+    <comment ref="G42" authorId="0">
+      <text>
+        <t>Correct Answer given</t>
+      </text>
+    </comment>
+    <comment ref="F43" authorId="0">
+      <text>
+        <t>Incorrect Answer given</t>
+      </text>
+    </comment>
+    <comment ref="H63" authorId="0">
+      <text>
+        <t>Correct Answer given</t>
+      </text>
+    </comment>
+    <comment ref="E21" authorId="0">
+      <text>
+        <t>Partially Correct Answer given</t>
+      </text>
+    </comment>
+    <comment ref="G41" authorId="0">
+      <text>
+        <t>Correct Answer given</t>
+      </text>
+    </comment>
+    <comment ref="F42" authorId="0">
+      <text>
+        <t>Correct Answer given</t>
+      </text>
+    </comment>
+    <comment ref="E43" authorId="0">
+      <text>
+        <t>Correct Answer given</t>
+      </text>
+    </comment>
+    <comment ref="H62" authorId="0">
+      <text>
+        <t>Correct Answer given</t>
+      </text>
+    </comment>
+    <comment ref="G43" authorId="0">
+      <text>
+        <t>Correct Answer given</t>
+      </text>
+    </comment>
+    <comment ref="E48" authorId="0">
+      <text>
+        <t>Correct Answer given</t>
+      </text>
+    </comment>
+    <comment ref="E47" authorId="0">
+      <text>
+        <t>Correct Answer given</t>
+      </text>
+    </comment>
+    <comment ref="G48" authorId="0">
+      <text>
+        <t>Correct Answer given</t>
+      </text>
+    </comment>
+    <comment ref="G47" authorId="0">
+      <text>
+        <t>Correct Answer given</t>
+      </text>
+    </comment>
+    <comment ref="E49" authorId="0">
+      <text>
+        <t>Correct Answer given</t>
+      </text>
+    </comment>
+    <comment ref="H49" authorId="0">
+      <text>
+        <t>Correct Answer given</t>
+      </text>
+    </comment>
+    <comment ref="G49" authorId="0">
+      <text>
+        <t>Correct Answer given</t>
+      </text>
+    </comment>
+    <comment ref="E6" authorId="0">
+      <text>
+        <t>Partially Correct Answer given</t>
+      </text>
+    </comment>
+    <comment ref="E7" authorId="0">
+      <text>
+        <t>Partially Correct Answer given</t>
+      </text>
+    </comment>
+    <comment ref="E8" authorId="0">
+      <text>
+        <t>Partially Correct Answer given</t>
+      </text>
+    </comment>
+    <comment ref="E9" authorId="0">
+      <text>
+        <t>Partially Correct Answer given</t>
+      </text>
+    </comment>
+    <comment ref="E11" authorId="0">
+      <text>
+        <t>Partially Correct Answer given</t>
+      </text>
+    </comment>
+    <comment ref="H52" authorId="0">
+      <text>
+        <t>Correct Answer given</t>
+      </text>
+    </comment>
+    <comment ref="E10" authorId="0">
+      <text>
+        <t>Partially Correct Answer given</t>
+      </text>
+    </comment>
+    <comment ref="B36" authorId="0">
+      <text>
+        <t>Correct Answer given</t>
+      </text>
+    </comment>
+    <comment ref="B37" authorId="0">
+      <text>
+        <t>Correct Answer given</t>
+      </text>
+    </comment>
+    <comment ref="H54" authorId="0">
+      <text>
+        <t>Correct Answer given</t>
+      </text>
+    </comment>
+    <comment ref="E12" authorId="0">
+      <text>
+        <t>Partially Correct Answer given</t>
+      </text>
+    </comment>
+    <comment ref="B38" authorId="0">
+      <text>
+        <t>Correct Answer given</t>
+      </text>
+    </comment>
+    <comment ref="H53" authorId="0">
+      <text>
+        <t>Correct Answer given</t>
+      </text>
+    </comment>
+    <comment ref="E15" authorId="0">
+      <text>
+        <t>Incorrect Answer given</t>
+      </text>
+    </comment>
+    <comment ref="E17" authorId="0">
+      <text>
+        <t>Partially Correct Answer given</t>
+      </text>
+    </comment>
+    <comment ref="H58" authorId="0">
+      <text>
+        <t>Correct Answer given</t>
+      </text>
+    </comment>
+    <comment ref="E16" authorId="0">
+      <text>
+        <t>Partially Correct Answer given</t>
+      </text>
+    </comment>
+    <comment ref="B41" authorId="0">
+      <text>
+        <t>Correct Answer given</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -186,7 +421,7 @@
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="144">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -245,8 +480,683 @@
       <name val="Liberation Sans"/>
       <family val="2"/>
     </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="45"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="48"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="45"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="48"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="45"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="48"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="45"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="48"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="45"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="48"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="45"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="48"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="45"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="48"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="45"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="48"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="45"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="48"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="45"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="48"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="45"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="48"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="45"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="48"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="45"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="48"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="45"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="48"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="45"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="48"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="45"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="48"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="45"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="48"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="45"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="48"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="45"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="48"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="45"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="48"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="45"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="48"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="45"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="48"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="45"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="48"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="45"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="48"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="45"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="48"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="45"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="48"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="45"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="48"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="45"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="48"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="45"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="48"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="45"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="48"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="45"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="48"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="45"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="48"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="45"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="48"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="45"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="48"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="45"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="48"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="45"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="48"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="45"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="48"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="45"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="48"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="45"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="48"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="45"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="48"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="45"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="48"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="45"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="48"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="45"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="48"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="45"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="48"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="45"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="48"/>
+    </font>
   </fonts>
-  <fills count="13">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -279,12 +1189,12 @@
     </fill>
     <fill>
       <patternFill patternType="none">
-        <fgColor indexed="10"/>
+        <fgColor indexed="45"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="10"/>
+        <fgColor indexed="45"/>
       </patternFill>
     </fill>
     <fill>
@@ -293,28 +1203,34 @@
       </patternFill>
     </fill>
     <fill>
-      <patternFill patternType="solid">
+      <patternFill patternType="mediumGray">
         <fgColor indexed="42"/>
       </patternFill>
     </fill>
     <fill>
+      <patternFill patternType="mediumGray">
+        <fgColor indexed="42"/>
+        <bgColor indexed="42"/>
+      </patternFill>
+    </fill>
+    <fill>
       <patternFill patternType="none">
-        <fgColor indexed="48"/>
+        <fgColor indexed="40"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="48"/>
+        <fgColor indexed="40"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="48"/>
-        <bgColor indexed="48"/>
+        <fgColor indexed="40"/>
+        <bgColor indexed="40"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="24">
+  <borders count="34">
     <border>
       <left/>
       <right/>
@@ -565,6 +1481,66 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin">
+        <color indexed="45"/>
+      </bottom>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin">
+        <color indexed="45"/>
+      </bottom>
+    </border>
+    <border>
+      <top style="thin">
+        <color indexed="45"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="45"/>
+      </bottom>
+    </border>
+    <border>
+      <bottom style="thin">
+        <color indexed="17"/>
+      </bottom>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin">
+        <color indexed="17"/>
+      </bottom>
+    </border>
+    <border>
+      <top style="thin">
+        <color indexed="17"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="17"/>
+      </bottom>
+    </border>
+    <border>
+      <bottom style="thin">
+        <color indexed="48"/>
+      </bottom>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin">
+        <color indexed="48"/>
+      </bottom>
+    </border>
+    <border>
+      <top style="thin">
+        <color indexed="48"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="48"/>
+      </bottom>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -847,141 +1823,141 @@
     <xf numFmtId="164" fontId="4" fillId="5" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="27" xfId="0" applyFill="true" applyFont="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="30" xfId="0" applyFill="true" applyFont="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="33" xfId="0" applyFill="true" applyFont="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="27" xfId="0" applyFill="true" applyFont="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="30" xfId="0" applyFill="true" applyFont="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="33" xfId="0" applyFill="true" applyFont="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="27" xfId="0" applyFill="true" applyFont="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="30" xfId="0" applyFill="true" applyFont="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="33" xfId="0" applyFill="true" applyFont="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="27" xfId="0" applyFill="true" applyFont="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="30" xfId="0" applyFill="true" applyFont="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="33" xfId="0" applyFill="true" applyFont="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="21" fillId="7" borderId="27" xfId="0" applyFill="true" applyFont="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="22" fillId="10" borderId="30" xfId="0" applyFill="true" applyFont="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="23" fillId="13" borderId="33" xfId="0" applyFill="true" applyFont="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="24" fillId="7" borderId="27" xfId="0" applyFill="true" applyFont="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="25" fillId="10" borderId="30" xfId="0" applyFill="true" applyFont="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="26" fillId="13" borderId="33" xfId="0" applyFill="true" applyFont="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="27" fillId="7" borderId="27" xfId="0" applyFill="true" applyFont="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="28" fillId="10" borderId="30" xfId="0" applyFill="true" applyFont="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="29" fillId="13" borderId="33" xfId="0" applyFill="true" applyFont="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="30" fillId="7" borderId="27" xfId="0" applyFill="true" applyFont="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="31" fillId="10" borderId="30" xfId="0" applyFill="true" applyFont="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="32" fillId="13" borderId="33" xfId="0" applyFill="true" applyFont="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="33" fillId="7" borderId="27" xfId="0" applyFill="true" applyFont="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="34" fillId="10" borderId="30" xfId="0" applyFill="true" applyFont="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="35" fillId="13" borderId="33" xfId="0" applyFill="true" applyFont="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="36" fillId="7" borderId="27" xfId="0" applyFill="true" applyFont="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="37" fillId="10" borderId="30" xfId="0" applyFill="true" applyFont="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="38" fillId="13" borderId="33" xfId="0" applyFill="true" applyFont="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="39" fillId="7" borderId="27" xfId="0" applyFill="true" applyFont="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="40" fillId="10" borderId="30" xfId="0" applyFill="true" applyFont="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="41" fillId="13" borderId="33" xfId="0" applyFill="true" applyFont="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="42" fillId="7" borderId="27" xfId="0" applyFill="true" applyFont="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="43" fillId="10" borderId="30" xfId="0" applyFill="true" applyFont="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="44" fillId="13" borderId="33" xfId="0" applyFill="true" applyFont="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="45" fillId="7" borderId="27" xfId="0" applyFill="true" applyFont="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="46" fillId="10" borderId="30" xfId="0" applyFill="true" applyFont="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="47" fillId="13" borderId="33" xfId="0" applyFill="true" applyFont="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="48" fillId="7" borderId="27" xfId="0" applyFill="true" applyFont="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="49" fillId="10" borderId="30" xfId="0" applyFill="true" applyFont="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="50" fillId="13" borderId="33" xfId="0" applyFill="true" applyFont="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="51" fillId="7" borderId="27" xfId="0" applyFill="true" applyFont="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="52" fillId="10" borderId="30" xfId="0" applyFill="true" applyFont="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="53" fillId="13" borderId="33" xfId="0" applyFill="true" applyFont="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="54" fillId="7" borderId="27" xfId="0" applyFill="true" applyFont="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="55" fillId="10" borderId="30" xfId="0" applyFill="true" applyFont="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="56" fillId="13" borderId="33" xfId="0" applyFill="true" applyFont="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="57" fillId="7" borderId="27" xfId="0" applyFill="true" applyFont="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="58" fillId="10" borderId="30" xfId="0" applyFill="true" applyFont="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="59" fillId="13" borderId="33" xfId="0" applyFill="true" applyFont="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="60" fillId="7" borderId="27" xfId="0" applyFill="true" applyFont="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="61" fillId="10" borderId="30" xfId="0" applyFill="true" applyFont="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="62" fillId="13" borderId="33" xfId="0" applyFill="true" applyFont="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="63" fillId="7" borderId="27" xfId="0" applyFill="true" applyFont="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="64" fillId="10" borderId="30" xfId="0" applyFill="true" applyFont="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="65" fillId="13" borderId="33" xfId="0" applyFill="true" applyFont="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="66" fillId="7" borderId="27" xfId="0" applyFill="true" applyFont="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="67" fillId="10" borderId="30" xfId="0" applyFill="true" applyFont="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="68" fillId="13" borderId="33" xfId="0" applyFill="true" applyFont="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="69" fillId="7" borderId="27" xfId="0" applyFill="true" applyFont="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="70" fillId="10" borderId="30" xfId="0" applyFill="true" applyFont="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="71" fillId="13" borderId="33" xfId="0" applyFill="true" applyFont="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="72" fillId="7" borderId="27" xfId="0" applyFill="true" applyFont="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="73" fillId="10" borderId="30" xfId="0" applyFill="true" applyFont="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="74" fillId="13" borderId="33" xfId="0" applyFill="true" applyFont="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="75" fillId="7" borderId="27" xfId="0" applyFill="true" applyFont="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="76" fillId="10" borderId="30" xfId="0" applyFill="true" applyFont="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="77" fillId="13" borderId="33" xfId="0" applyFill="true" applyFont="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="78" fillId="7" borderId="27" xfId="0" applyFill="true" applyFont="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="79" fillId="10" borderId="30" xfId="0" applyFill="true" applyFont="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="80" fillId="13" borderId="33" xfId="0" applyFill="true" applyFont="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="81" fillId="7" borderId="27" xfId="0" applyFill="true" applyFont="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="82" fillId="10" borderId="30" xfId="0" applyFill="true" applyFont="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="83" fillId="13" borderId="33" xfId="0" applyFill="true" applyFont="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="84" fillId="7" borderId="27" xfId="0" applyFill="true" applyFont="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="85" fillId="10" borderId="30" xfId="0" applyFill="true" applyFont="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="86" fillId="13" borderId="33" xfId="0" applyFill="true" applyFont="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="87" fillId="7" borderId="27" xfId="0" applyFill="true" applyFont="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="88" fillId="10" borderId="30" xfId="0" applyFill="true" applyFont="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="89" fillId="13" borderId="33" xfId="0" applyFill="true" applyFont="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="90" fillId="7" borderId="27" xfId="0" applyFill="true" applyFont="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="91" fillId="10" borderId="30" xfId="0" applyFill="true" applyFont="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="92" fillId="13" borderId="33" xfId="0" applyFill="true" applyFont="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="93" fillId="7" borderId="27" xfId="0" applyFill="true" applyFont="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="94" fillId="10" borderId="30" xfId="0" applyFill="true" applyFont="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="95" fillId="13" borderId="33" xfId="0" applyFill="true" applyFont="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="96" fillId="7" borderId="27" xfId="0" applyFill="true" applyFont="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="97" fillId="10" borderId="30" xfId="0" applyFill="true" applyFont="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="98" fillId="13" borderId="33" xfId="0" applyFill="true" applyFont="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="99" fillId="7" borderId="27" xfId="0" applyFill="true" applyFont="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="100" fillId="10" borderId="30" xfId="0" applyFill="true" applyFont="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="101" fillId="13" borderId="33" xfId="0" applyFill="true" applyFont="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="102" fillId="7" borderId="27" xfId="0" applyFill="true" applyFont="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="103" fillId="10" borderId="30" xfId="0" applyFill="true" applyFont="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="104" fillId="13" borderId="33" xfId="0" applyFill="true" applyFont="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="105" fillId="7" borderId="27" xfId="0" applyFill="true" applyFont="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="106" fillId="10" borderId="30" xfId="0" applyFill="true" applyFont="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="107" fillId="13" borderId="33" xfId="0" applyFill="true" applyFont="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="108" fillId="7" borderId="27" xfId="0" applyFill="true" applyFont="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="109" fillId="10" borderId="30" xfId="0" applyFill="true" applyFont="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="110" fillId="13" borderId="33" xfId="0" applyFill="true" applyFont="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="111" fillId="7" borderId="27" xfId="0" applyFill="true" applyFont="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="112" fillId="10" borderId="30" xfId="0" applyFill="true" applyFont="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="113" fillId="13" borderId="33" xfId="0" applyFill="true" applyFont="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="114" fillId="7" borderId="27" xfId="0" applyFill="true" applyFont="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="115" fillId="10" borderId="30" xfId="0" applyFill="true" applyFont="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="116" fillId="13" borderId="33" xfId="0" applyFill="true" applyFont="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="117" fillId="7" borderId="27" xfId="0" applyFill="true" applyFont="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="118" fillId="10" borderId="30" xfId="0" applyFill="true" applyFont="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="119" fillId="13" borderId="33" xfId="0" applyFill="true" applyFont="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="120" fillId="7" borderId="27" xfId="0" applyFill="true" applyFont="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="121" fillId="10" borderId="30" xfId="0" applyFill="true" applyFont="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="122" fillId="13" borderId="33" xfId="0" applyFill="true" applyFont="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="123" fillId="7" borderId="27" xfId="0" applyFill="true" applyFont="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="124" fillId="10" borderId="30" xfId="0" applyFill="true" applyFont="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="125" fillId="13" borderId="33" xfId="0" applyFill="true" applyFont="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="126" fillId="7" borderId="27" xfId="0" applyFill="true" applyFont="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="127" fillId="10" borderId="30" xfId="0" applyFill="true" applyFont="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="128" fillId="13" borderId="33" xfId="0" applyFill="true" applyFont="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="129" fillId="7" borderId="27" xfId="0" applyFill="true" applyFont="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="130" fillId="10" borderId="30" xfId="0" applyFill="true" applyFont="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="131" fillId="13" borderId="33" xfId="0" applyFill="true" applyFont="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="132" fillId="7" borderId="27" xfId="0" applyFill="true" applyFont="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="133" fillId="10" borderId="30" xfId="0" applyFill="true" applyFont="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="134" fillId="13" borderId="33" xfId="0" applyFill="true" applyFont="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="135" fillId="7" borderId="27" xfId="0" applyFill="true" applyFont="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="136" fillId="10" borderId="30" xfId="0" applyFill="true" applyFont="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="137" fillId="13" borderId="33" xfId="0" applyFill="true" applyFont="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="138" fillId="7" borderId="27" xfId="0" applyFill="true" applyFont="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="139" fillId="10" borderId="30" xfId="0" applyFill="true" applyFont="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="140" fillId="13" borderId="33" xfId="0" applyFill="true" applyFont="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="141" fillId="7" borderId="27" xfId="0" applyFill="true" applyFont="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="142" fillId="10" borderId="30" xfId="0" applyFill="true" applyFont="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="143" fillId="13" borderId="33" xfId="0" applyFill="true" applyFont="true" applyBorder="true"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1006,6 +1982,1227 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="1" name="Picture 1" descr="Picture"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="true"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="152400" cy="152400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1" descr="Picture"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="true"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="152400" cy="152400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 1" descr="Picture"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="true"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="152400" cy="152400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 1" descr="Picture"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="true"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="152400" cy="152400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 1" descr="Picture"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="true"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="152400" cy="152400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 1" descr="Picture"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="true"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="152400" cy="152400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 1" descr="Picture"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="true"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="152400" cy="152400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 1" descr="Picture"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="true"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId8"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="152400" cy="152400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 1" descr="Picture"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="true"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId9"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="152400" cy="152400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Picture 1" descr="Picture"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="true"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId10"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="152400" cy="152400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Picture 1" descr="Picture"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="true"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId11"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="152400" cy="152400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="Picture 1" descr="Picture"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="true"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId12"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="152400" cy="152400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="Picture 1" descr="Picture"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="true"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId13"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="152400" cy="152400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="14" name="Picture 1" descr="Picture"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="true"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId14"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="152400" cy="152400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="15" name="Picture 1" descr="Picture"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="true"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId15"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="152400" cy="152400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="16" name="Picture 1" descr="Picture"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="true"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId16"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="152400" cy="152400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="17" name="Picture 1" descr="Picture"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="true"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId17"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="152400" cy="152400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="18" name="Picture 1" descr="Picture"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="true"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId18"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="152400" cy="152400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="19" name="Picture 1" descr="Picture"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="true"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId19"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="152400" cy="152400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="20" name="Picture 1" descr="Picture"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="true"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId20"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="152400" cy="152400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="21" name="Picture 1" descr="Picture"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="true"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId21"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="152400" cy="152400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="22" name="Picture 1" descr="Picture"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="true"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId22"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="152400" cy="152400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="23" name="Picture 1" descr="Picture"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="true"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId23"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="152400" cy="152400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="24" name="Picture 1" descr="Picture"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="true"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId24"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="152400" cy="152400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="25" name="Picture 1" descr="Picture"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="true"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId25"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="152400" cy="152400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="26" name="Picture 1" descr="Picture"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="true"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId26"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="152400" cy="152400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="27" name="Picture 1" descr="Picture"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="true"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId27"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="152400" cy="152400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="28" name="Picture 1" descr="Picture"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="true"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId28"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="152400" cy="152400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="29" name="Picture 1" descr="Picture"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="true"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId29"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="152400" cy="152400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="30" name="Picture 1" descr="Picture"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="true"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId30"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="152400" cy="152400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="31" name="Picture 1" descr="Picture"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="true"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId31"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="152400" cy="152400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="32" name="Picture 1" descr="Picture"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="true"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId32"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="152400" cy="152400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2216,6 +4413,8 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId4"/>
 </worksheet>
 </file>
 

</xml_diff>